<commit_message>
Updated ESD1 excel file again to fix issue
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_esd1.xlsx
+++ b/andes/cases/ieee14/ieee14_esd1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trey0\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5596299-ADA5-483F-B209-4C2755942B8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EF4E16-96DD-423A-A27C-DE74159857CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="10" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="263">
   <si>
     <t>uid</t>
   </si>
@@ -798,18 +798,55 @@
   </si>
   <si>
     <t>SOCinit</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>3a</t>
+  </si>
+  <si>
+    <t>4a</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>6a</t>
+  </si>
+  <si>
+    <t>7a</t>
+  </si>
+  <si>
+    <t>8a</t>
+  </si>
+  <si>
+    <t>9a</t>
+  </si>
+  <si>
+    <t>10a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -864,12 +901,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3340,9 +3378,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AH11"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:AH11"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -4555,8 +4593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02DC62D-3467-4D6F-BA2E-7B4F29F7DD6F}">
   <dimension ref="A1:AL11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AL2" sqref="AL2:AL11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4681,8 +4719,8 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4794,8 +4832,8 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" s="3" t="s">
+        <v>254</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -4907,8 +4945,8 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="B4" s="3" t="s">
+        <v>255</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -5020,8 +5058,8 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>4</v>
+      <c r="B5" s="3" t="s">
+        <v>256</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -5133,8 +5171,8 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>5</v>
+      <c r="B6" s="3" t="s">
+        <v>257</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -5246,8 +5284,8 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>6</v>
+      <c r="B7" s="3" t="s">
+        <v>258</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5359,8 +5397,8 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>7</v>
+      <c r="B8" s="3" t="s">
+        <v>259</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -5472,8 +5510,8 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>8</v>
+      <c r="B9" s="3" t="s">
+        <v>260</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -5585,8 +5623,8 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>9</v>
+      <c r="B10" s="3" t="s">
+        <v>261</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -5698,8 +5736,8 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>10</v>
+      <c r="B11" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="C11">
         <v>1</v>

</xml_diff>

<commit_message>
Updated ESD1 test case.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_esd1.xlsx
+++ b/andes/cases/ieee14/ieee14_esd1.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trey0\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EF4E16-96DD-423A-A27C-DE74159857CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="10" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="21540" windowHeight="8235" firstSheet="11" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -31,15 +25,14 @@
     <sheet name="IEEEST" sheetId="16" r:id="rId16"/>
     <sheet name="ST2CUT" sheetId="17" r:id="rId17"/>
     <sheet name="BusFreq" sheetId="18" r:id="rId18"/>
-    <sheet name="PVD1" sheetId="19" r:id="rId19"/>
-    <sheet name="ESD1" sheetId="20" r:id="rId20"/>
+    <sheet name="ESD1" sheetId="20" r:id="rId19"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="253">
   <si>
     <t>uid</t>
   </si>
@@ -761,36 +754,6 @@
     <t>gammaq</t>
   </si>
   <si>
-    <t>PVD1_1</t>
-  </si>
-  <si>
-    <t>PVD1_2</t>
-  </si>
-  <si>
-    <t>PVD1_3</t>
-  </si>
-  <si>
-    <t>PVD1_4</t>
-  </si>
-  <si>
-    <t>PVD1_5</t>
-  </si>
-  <si>
-    <t>PVD1_6</t>
-  </si>
-  <si>
-    <t>PVD1_7</t>
-  </si>
-  <si>
-    <t>PVD1_8</t>
-  </si>
-  <si>
-    <t>PVD1_9</t>
-  </si>
-  <si>
-    <t>PVD1_10</t>
-  </si>
-  <si>
     <t>SOCmin</t>
   </si>
   <si>
@@ -800,53 +763,52 @@
     <t>SOCinit</t>
   </si>
   <si>
-    <t>1a</t>
-  </si>
-  <si>
-    <t>2a</t>
-  </si>
-  <si>
-    <t>3a</t>
-  </si>
-  <si>
-    <t>4a</t>
-  </si>
-  <si>
-    <t>5a</t>
-  </si>
-  <si>
-    <t>6a</t>
-  </si>
-  <si>
-    <t>7a</t>
-  </si>
-  <si>
-    <t>8a</t>
-  </si>
-  <si>
-    <t>9a</t>
-  </si>
-  <si>
-    <t>10a</t>
+    <t>ESD1_1</t>
+  </si>
+  <si>
+    <t>ESD1_2</t>
+  </si>
+  <si>
+    <t>ESD1_3</t>
+  </si>
+  <si>
+    <t>ESD1_4</t>
+  </si>
+  <si>
+    <t>ESD1_5</t>
+  </si>
+  <si>
+    <t>ESD1_6</t>
+  </si>
+  <si>
+    <t>ESD1_7</t>
+  </si>
+  <si>
+    <t>ESD1_8</t>
+  </si>
+  <si>
+    <t>ESD1_9</t>
+  </si>
+  <si>
+    <t>ESD1_10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -858,23 +820,360 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -897,29 +1196,315 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1204,20 +1789,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -1243,19 +1829,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="6"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
@@ -1305,19 +1894,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
@@ -1550,13 +2142,13 @@
         <v>1.75</v>
       </c>
       <c r="V3">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="W3">
         <v>0.8</v>
       </c>
       <c r="X3">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="Y3">
         <v>6.5</v>
@@ -1716,13 +2308,13 @@
         <v>1.75</v>
       </c>
       <c r="V5">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="W5">
         <v>0.8</v>
       </c>
       <c r="X5">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="Y5">
         <v>6.5</v>
@@ -1822,19 +2414,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
@@ -2005,19 +2600,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
@@ -2176,7 +2774,7 @@
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>8.7200000000000006</v>
+        <v>8.72</v>
       </c>
       <c r="AA2">
         <v>0.7</v>
@@ -2256,7 +2854,7 @@
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>8.7200000000000006</v>
+        <v>8.72</v>
       </c>
       <c r="AA3">
         <v>0.7</v>
@@ -2267,19 +2865,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
@@ -2389,19 +2990,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4"/>
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
@@ -2545,7 +3149,7 @@
         <v>0.01</v>
       </c>
       <c r="U2">
-        <v>9.7999999999999997E-3</v>
+        <v>0.0098</v>
       </c>
       <c r="V2">
         <v>3.86</v>
@@ -2625,7 +3229,7 @@
         <v>0.01</v>
       </c>
       <c r="U3">
-        <v>9.7999999999999997E-3</v>
+        <v>0.0098</v>
       </c>
       <c r="V3">
         <v>3.86</v>
@@ -2705,7 +3309,7 @@
         <v>0.01</v>
       </c>
       <c r="U4">
-        <v>9.7999999999999997E-3</v>
+        <v>0.0098</v>
       </c>
       <c r="V4">
         <v>3.86</v>
@@ -2785,7 +3389,7 @@
         <v>0.01</v>
       </c>
       <c r="U5">
-        <v>9.7999999999999997E-3</v>
+        <v>0.0098</v>
       </c>
       <c r="V5">
         <v>3.86</v>
@@ -2805,19 +3409,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
@@ -2972,19 +3579,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <sheetData>
     <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
@@ -3119,13 +3729,13 @@
         <v>0.23</v>
       </c>
       <c r="S2">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="T2">
         <v>0.23</v>
       </c>
       <c r="U2">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -3225,19 +3835,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4" outlineLevelCol="7"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
@@ -3371,21 +3984,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:AH11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:AL11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3488,19 +4102,31 @@
       <c r="AH1" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="2" spans="1:34">
+      <c r="AI1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -3533,19 +4159,19 @@
         <v>0.8</v>
       </c>
       <c r="P2">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="Q2">
         <v>-1</v>
       </c>
       <c r="R2">
-        <v>-1.7000000000000001E-2</v>
+        <v>-0.017</v>
       </c>
       <c r="S2">
         <v>5</v>
       </c>
       <c r="T2">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="U2">
         <v>0.88</v>
@@ -3554,7 +4180,7 @@
         <v>0.9</v>
       </c>
       <c r="W2">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="X2">
         <v>1.2</v>
@@ -3589,19 +4215,31 @@
       <c r="AH2">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:34">
+      <c r="AI2">
+        <v>1</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AL2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -3634,19 +4272,19 @@
         <v>0.8</v>
       </c>
       <c r="P3">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="Q3">
         <v>-1</v>
       </c>
       <c r="R3">
-        <v>-1.7000000000000001E-2</v>
+        <v>-0.017</v>
       </c>
       <c r="S3">
         <v>5</v>
       </c>
       <c r="T3">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="U3">
         <v>0.88</v>
@@ -3655,7 +4293,7 @@
         <v>0.9</v>
       </c>
       <c r="W3">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="X3">
         <v>1.2</v>
@@ -3690,19 +4328,31 @@
       <c r="AH3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:34">
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -3735,19 +4385,19 @@
         <v>0.8</v>
       </c>
       <c r="P4">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="Q4">
         <v>-1</v>
       </c>
       <c r="R4">
-        <v>-1.7000000000000001E-2</v>
+        <v>-0.017</v>
       </c>
       <c r="S4">
         <v>5</v>
       </c>
       <c r="T4">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="U4">
         <v>0.88</v>
@@ -3756,7 +4406,7 @@
         <v>0.9</v>
       </c>
       <c r="W4">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="X4">
         <v>1.2</v>
@@ -3791,19 +4441,31 @@
       <c r="AH4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:34">
+      <c r="AI4">
+        <v>1</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>1</v>
+      </c>
+      <c r="AL4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -3836,19 +4498,19 @@
         <v>0.8</v>
       </c>
       <c r="P5">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="Q5">
         <v>-1</v>
       </c>
       <c r="R5">
-        <v>-1.7000000000000001E-2</v>
+        <v>-0.017</v>
       </c>
       <c r="S5">
         <v>5</v>
       </c>
       <c r="T5">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="U5">
         <v>0.88</v>
@@ -3857,7 +4519,7 @@
         <v>0.9</v>
       </c>
       <c r="W5">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="X5">
         <v>1.2</v>
@@ -3892,19 +4554,31 @@
       <c r="AH5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:34">
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AL5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>5</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -3937,19 +4611,19 @@
         <v>0.8</v>
       </c>
       <c r="P6">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="Q6">
         <v>-1</v>
       </c>
       <c r="R6">
-        <v>-1.7000000000000001E-2</v>
+        <v>-0.017</v>
       </c>
       <c r="S6">
         <v>5</v>
       </c>
       <c r="T6">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="U6">
         <v>0.88</v>
@@ -3958,7 +4632,7 @@
         <v>0.9</v>
       </c>
       <c r="W6">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="X6">
         <v>1.2</v>
@@ -3993,19 +4667,31 @@
       <c r="AH6">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="7" spans="1:34">
+      <c r="AI6">
+        <v>1</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>1</v>
+      </c>
+      <c r="AL6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>6</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -4038,19 +4724,19 @@
         <v>0.8</v>
       </c>
       <c r="P7">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="Q7">
         <v>-1</v>
       </c>
       <c r="R7">
-        <v>-1.7000000000000001E-2</v>
+        <v>-0.017</v>
       </c>
       <c r="S7">
         <v>5</v>
       </c>
       <c r="T7">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="U7">
         <v>0.88</v>
@@ -4059,7 +4745,7 @@
         <v>0.9</v>
       </c>
       <c r="W7">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="X7">
         <v>1.2</v>
@@ -4094,19 +4780,31 @@
       <c r="AH7">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:34">
+      <c r="AI7">
+        <v>1</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>1</v>
+      </c>
+      <c r="AL7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>7</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -4139,19 +4837,19 @@
         <v>0.8</v>
       </c>
       <c r="P8">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="Q8">
         <v>-1</v>
       </c>
       <c r="R8">
-        <v>-1.7000000000000001E-2</v>
+        <v>-0.017</v>
       </c>
       <c r="S8">
         <v>5</v>
       </c>
       <c r="T8">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="U8">
         <v>0.88</v>
@@ -4160,7 +4858,7 @@
         <v>0.9</v>
       </c>
       <c r="W8">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="X8">
         <v>1.2</v>
@@ -4195,19 +4893,31 @@
       <c r="AH8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="9" spans="1:34">
+      <c r="AI8">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>8</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -4240,19 +4950,19 @@
         <v>0.8</v>
       </c>
       <c r="P9">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="Q9">
         <v>-1</v>
       </c>
       <c r="R9">
-        <v>-1.7000000000000001E-2</v>
+        <v>-0.017</v>
       </c>
       <c r="S9">
         <v>5</v>
       </c>
       <c r="T9">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="U9">
         <v>0.88</v>
@@ -4261,7 +4971,7 @@
         <v>0.9</v>
       </c>
       <c r="W9">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="X9">
         <v>1.2</v>
@@ -4296,19 +5006,31 @@
       <c r="AH9">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:34">
+      <c r="AI9">
+        <v>1</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>9</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -4341,19 +5063,19 @@
         <v>0.8</v>
       </c>
       <c r="P10">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="Q10">
         <v>-1</v>
       </c>
       <c r="R10">
-        <v>-1.7000000000000001E-2</v>
+        <v>-0.017</v>
       </c>
       <c r="S10">
         <v>5</v>
       </c>
       <c r="T10">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="U10">
         <v>0.88</v>
@@ -4362,7 +5084,7 @@
         <v>0.9</v>
       </c>
       <c r="W10">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="X10">
         <v>1.2</v>
@@ -4397,19 +5119,31 @@
       <c r="AH10">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:34">
+      <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AL10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>10</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -4442,19 +5176,19 @@
         <v>0.8</v>
       </c>
       <c r="P11">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="Q11">
         <v>-1</v>
       </c>
       <c r="R11">
-        <v>-1.7000000000000001E-2</v>
+        <v>-0.017</v>
       </c>
       <c r="S11">
         <v>5</v>
       </c>
       <c r="T11">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="U11">
         <v>0.88</v>
@@ -4463,7 +5197,7 @@
         <v>0.9</v>
       </c>
       <c r="W11">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="X11">
         <v>1.2</v>
@@ -4498,22 +5232,38 @@
       <c r="AH11">
         <v>0.1</v>
       </c>
+      <c r="AI11">
+        <v>1</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>1</v>
+      </c>
+      <c r="AL11">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="6"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
@@ -4586,1281 +5336,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02DC62D-3467-4D6F-BA2E-7B4F29F7DD6F}">
-  <dimension ref="A1:AL11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:38">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>60</v>
-      </c>
-      <c r="I2" t="s">
-        <v>215</v>
-      </c>
-      <c r="J2">
-        <v>0.01</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>0.33</v>
-      </c>
-      <c r="N2">
-        <v>-0.33</v>
-      </c>
-      <c r="O2">
-        <v>0.8</v>
-      </c>
-      <c r="P2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q2">
-        <v>-1</v>
-      </c>
-      <c r="R2">
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="S2">
-        <v>5</v>
-      </c>
-      <c r="T2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U2">
-        <v>0.88</v>
-      </c>
-      <c r="V2">
-        <v>0.9</v>
-      </c>
-      <c r="W2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="X2">
-        <v>1.2</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>59.5</v>
-      </c>
-      <c r="AA2">
-        <v>59.7</v>
-      </c>
-      <c r="AB2">
-        <v>60.3</v>
-      </c>
-      <c r="AC2">
-        <v>60.5</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>0.02</v>
-      </c>
-      <c r="AF2">
-        <v>0.02</v>
-      </c>
-      <c r="AG2">
-        <v>0.1</v>
-      </c>
-      <c r="AH2">
-        <v>0.1</v>
-      </c>
-      <c r="AI2">
-        <v>1</v>
-      </c>
-      <c r="AJ2">
-        <v>0</v>
-      </c>
-      <c r="AK2">
-        <v>1</v>
-      </c>
-      <c r="AL2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>60</v>
-      </c>
-      <c r="I3" t="s">
-        <v>215</v>
-      </c>
-      <c r="J3">
-        <v>0.01</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>0.33</v>
-      </c>
-      <c r="N3">
-        <v>-0.33</v>
-      </c>
-      <c r="O3">
-        <v>0.8</v>
-      </c>
-      <c r="P3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q3">
-        <v>-1</v>
-      </c>
-      <c r="R3">
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="S3">
-        <v>5</v>
-      </c>
-      <c r="T3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U3">
-        <v>0.88</v>
-      </c>
-      <c r="V3">
-        <v>0.9</v>
-      </c>
-      <c r="W3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="X3">
-        <v>1.2</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>59.5</v>
-      </c>
-      <c r="AA3">
-        <v>59.7</v>
-      </c>
-      <c r="AB3">
-        <v>60.3</v>
-      </c>
-      <c r="AC3">
-        <v>60.5</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>0.02</v>
-      </c>
-      <c r="AF3">
-        <v>0.02</v>
-      </c>
-      <c r="AG3">
-        <v>0.1</v>
-      </c>
-      <c r="AH3">
-        <v>0.1</v>
-      </c>
-      <c r="AI3">
-        <v>1</v>
-      </c>
-      <c r="AJ3">
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <v>1</v>
-      </c>
-      <c r="AL3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>242</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>60</v>
-      </c>
-      <c r="I4" t="s">
-        <v>215</v>
-      </c>
-      <c r="J4">
-        <v>0.01</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0.33</v>
-      </c>
-      <c r="N4">
-        <v>-0.33</v>
-      </c>
-      <c r="O4">
-        <v>0.8</v>
-      </c>
-      <c r="P4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q4">
-        <v>-1</v>
-      </c>
-      <c r="R4">
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="S4">
-        <v>5</v>
-      </c>
-      <c r="T4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U4">
-        <v>0.88</v>
-      </c>
-      <c r="V4">
-        <v>0.9</v>
-      </c>
-      <c r="W4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="X4">
-        <v>1.2</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>59.5</v>
-      </c>
-      <c r="AA4">
-        <v>59.7</v>
-      </c>
-      <c r="AB4">
-        <v>60.3</v>
-      </c>
-      <c r="AC4">
-        <v>60.5</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>0.02</v>
-      </c>
-      <c r="AF4">
-        <v>0.02</v>
-      </c>
-      <c r="AG4">
-        <v>0.1</v>
-      </c>
-      <c r="AH4">
-        <v>0.1</v>
-      </c>
-      <c r="AI4">
-        <v>1</v>
-      </c>
-      <c r="AJ4">
-        <v>0</v>
-      </c>
-      <c r="AK4">
-        <v>1</v>
-      </c>
-      <c r="AL4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>60</v>
-      </c>
-      <c r="I5" t="s">
-        <v>215</v>
-      </c>
-      <c r="J5">
-        <v>0.01</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0.33</v>
-      </c>
-      <c r="N5">
-        <v>-0.33</v>
-      </c>
-      <c r="O5">
-        <v>0.8</v>
-      </c>
-      <c r="P5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q5">
-        <v>-1</v>
-      </c>
-      <c r="R5">
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="S5">
-        <v>5</v>
-      </c>
-      <c r="T5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U5">
-        <v>0.88</v>
-      </c>
-      <c r="V5">
-        <v>0.9</v>
-      </c>
-      <c r="W5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="X5">
-        <v>1.2</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>59.5</v>
-      </c>
-      <c r="AA5">
-        <v>59.7</v>
-      </c>
-      <c r="AB5">
-        <v>60.3</v>
-      </c>
-      <c r="AC5">
-        <v>60.5</v>
-      </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5">
-        <v>0.02</v>
-      </c>
-      <c r="AF5">
-        <v>0.02</v>
-      </c>
-      <c r="AG5">
-        <v>0.1</v>
-      </c>
-      <c r="AH5">
-        <v>0.1</v>
-      </c>
-      <c r="AI5">
-        <v>1</v>
-      </c>
-      <c r="AJ5">
-        <v>0</v>
-      </c>
-      <c r="AK5">
-        <v>1</v>
-      </c>
-      <c r="AL5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>244</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>6</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>60</v>
-      </c>
-      <c r="I6" t="s">
-        <v>215</v>
-      </c>
-      <c r="J6">
-        <v>0.01</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>0.33</v>
-      </c>
-      <c r="N6">
-        <v>-0.33</v>
-      </c>
-      <c r="O6">
-        <v>0.8</v>
-      </c>
-      <c r="P6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q6">
-        <v>-1</v>
-      </c>
-      <c r="R6">
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="S6">
-        <v>5</v>
-      </c>
-      <c r="T6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U6">
-        <v>0.88</v>
-      </c>
-      <c r="V6">
-        <v>0.9</v>
-      </c>
-      <c r="W6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="X6">
-        <v>1.2</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>59.5</v>
-      </c>
-      <c r="AA6">
-        <v>59.7</v>
-      </c>
-      <c r="AB6">
-        <v>60.3</v>
-      </c>
-      <c r="AC6">
-        <v>60.5</v>
-      </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
-        <v>0.02</v>
-      </c>
-      <c r="AF6">
-        <v>0.02</v>
-      </c>
-      <c r="AG6">
-        <v>0.1</v>
-      </c>
-      <c r="AH6">
-        <v>0.1</v>
-      </c>
-      <c r="AI6">
-        <v>1</v>
-      </c>
-      <c r="AJ6">
-        <v>0</v>
-      </c>
-      <c r="AK6">
-        <v>1</v>
-      </c>
-      <c r="AL6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>245</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>60</v>
-      </c>
-      <c r="I7" t="s">
-        <v>215</v>
-      </c>
-      <c r="J7">
-        <v>0.01</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0.33</v>
-      </c>
-      <c r="N7">
-        <v>-0.33</v>
-      </c>
-      <c r="O7">
-        <v>0.8</v>
-      </c>
-      <c r="P7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q7">
-        <v>-1</v>
-      </c>
-      <c r="R7">
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="S7">
-        <v>5</v>
-      </c>
-      <c r="T7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U7">
-        <v>0.88</v>
-      </c>
-      <c r="V7">
-        <v>0.9</v>
-      </c>
-      <c r="W7">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="X7">
-        <v>1.2</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>59.5</v>
-      </c>
-      <c r="AA7">
-        <v>59.7</v>
-      </c>
-      <c r="AB7">
-        <v>60.3</v>
-      </c>
-      <c r="AC7">
-        <v>60.5</v>
-      </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7">
-        <v>0.02</v>
-      </c>
-      <c r="AF7">
-        <v>0.02</v>
-      </c>
-      <c r="AG7">
-        <v>0.1</v>
-      </c>
-      <c r="AH7">
-        <v>0.1</v>
-      </c>
-      <c r="AI7">
-        <v>1</v>
-      </c>
-      <c r="AJ7">
-        <v>0</v>
-      </c>
-      <c r="AK7">
-        <v>1</v>
-      </c>
-      <c r="AL7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>246</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <v>6</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>60</v>
-      </c>
-      <c r="I8" t="s">
-        <v>215</v>
-      </c>
-      <c r="J8">
-        <v>0.01</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0.33</v>
-      </c>
-      <c r="N8">
-        <v>-0.33</v>
-      </c>
-      <c r="O8">
-        <v>0.8</v>
-      </c>
-      <c r="P8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q8">
-        <v>-1</v>
-      </c>
-      <c r="R8">
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="S8">
-        <v>5</v>
-      </c>
-      <c r="T8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U8">
-        <v>0.88</v>
-      </c>
-      <c r="V8">
-        <v>0.9</v>
-      </c>
-      <c r="W8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="X8">
-        <v>1.2</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>59.5</v>
-      </c>
-      <c r="AA8">
-        <v>59.7</v>
-      </c>
-      <c r="AB8">
-        <v>60.3</v>
-      </c>
-      <c r="AC8">
-        <v>60.5</v>
-      </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
-      <c r="AE8">
-        <v>0.02</v>
-      </c>
-      <c r="AF8">
-        <v>0.02</v>
-      </c>
-      <c r="AG8">
-        <v>0.1</v>
-      </c>
-      <c r="AH8">
-        <v>0.1</v>
-      </c>
-      <c r="AI8">
-        <v>1</v>
-      </c>
-      <c r="AJ8">
-        <v>0</v>
-      </c>
-      <c r="AK8">
-        <v>1</v>
-      </c>
-      <c r="AL8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>247</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>6</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>60</v>
-      </c>
-      <c r="I9" t="s">
-        <v>215</v>
-      </c>
-      <c r="J9">
-        <v>0.01</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0.33</v>
-      </c>
-      <c r="N9">
-        <v>-0.33</v>
-      </c>
-      <c r="O9">
-        <v>0.8</v>
-      </c>
-      <c r="P9">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q9">
-        <v>-1</v>
-      </c>
-      <c r="R9">
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="S9">
-        <v>5</v>
-      </c>
-      <c r="T9">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U9">
-        <v>0.88</v>
-      </c>
-      <c r="V9">
-        <v>0.9</v>
-      </c>
-      <c r="W9">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="X9">
-        <v>1.2</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9">
-        <v>59.5</v>
-      </c>
-      <c r="AA9">
-        <v>59.7</v>
-      </c>
-      <c r="AB9">
-        <v>60.3</v>
-      </c>
-      <c r="AC9">
-        <v>60.5</v>
-      </c>
-      <c r="AD9">
-        <v>0</v>
-      </c>
-      <c r="AE9">
-        <v>0.02</v>
-      </c>
-      <c r="AF9">
-        <v>0.02</v>
-      </c>
-      <c r="AG9">
-        <v>0.1</v>
-      </c>
-      <c r="AH9">
-        <v>0.1</v>
-      </c>
-      <c r="AI9">
-        <v>1</v>
-      </c>
-      <c r="AJ9">
-        <v>0</v>
-      </c>
-      <c r="AK9">
-        <v>1</v>
-      </c>
-      <c r="AL9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>248</v>
-      </c>
-      <c r="E10">
-        <v>4</v>
-      </c>
-      <c r="F10">
-        <v>6</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>60</v>
-      </c>
-      <c r="I10" t="s">
-        <v>215</v>
-      </c>
-      <c r="J10">
-        <v>0.01</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0.33</v>
-      </c>
-      <c r="N10">
-        <v>-0.33</v>
-      </c>
-      <c r="O10">
-        <v>0.8</v>
-      </c>
-      <c r="P10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q10">
-        <v>-1</v>
-      </c>
-      <c r="R10">
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="S10">
-        <v>5</v>
-      </c>
-      <c r="T10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U10">
-        <v>0.88</v>
-      </c>
-      <c r="V10">
-        <v>0.9</v>
-      </c>
-      <c r="W10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="X10">
-        <v>1.2</v>
-      </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
-      <c r="Z10">
-        <v>59.5</v>
-      </c>
-      <c r="AA10">
-        <v>59.7</v>
-      </c>
-      <c r="AB10">
-        <v>60.3</v>
-      </c>
-      <c r="AC10">
-        <v>60.5</v>
-      </c>
-      <c r="AD10">
-        <v>0</v>
-      </c>
-      <c r="AE10">
-        <v>0.02</v>
-      </c>
-      <c r="AF10">
-        <v>0.02</v>
-      </c>
-      <c r="AG10">
-        <v>0.1</v>
-      </c>
-      <c r="AH10">
-        <v>0.1</v>
-      </c>
-      <c r="AI10">
-        <v>1</v>
-      </c>
-      <c r="AJ10">
-        <v>0</v>
-      </c>
-      <c r="AK10">
-        <v>1</v>
-      </c>
-      <c r="AL10">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:38">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>249</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11">
-        <v>6</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>60</v>
-      </c>
-      <c r="I11" t="s">
-        <v>215</v>
-      </c>
-      <c r="J11">
-        <v>0.01</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0.33</v>
-      </c>
-      <c r="N11">
-        <v>-0.33</v>
-      </c>
-      <c r="O11">
-        <v>0.8</v>
-      </c>
-      <c r="P11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q11">
-        <v>-1</v>
-      </c>
-      <c r="R11">
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="S11">
-        <v>5</v>
-      </c>
-      <c r="T11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U11">
-        <v>0.88</v>
-      </c>
-      <c r="V11">
-        <v>0.9</v>
-      </c>
-      <c r="W11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="X11">
-        <v>1.2</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <v>59.5</v>
-      </c>
-      <c r="AA11">
-        <v>59.7</v>
-      </c>
-      <c r="AB11">
-        <v>60.3</v>
-      </c>
-      <c r="AC11">
-        <v>60.5</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <v>0.02</v>
-      </c>
-      <c r="AF11">
-        <v>0.02</v>
-      </c>
-      <c r="AG11">
-        <v>0.1</v>
-      </c>
-      <c r="AH11">
-        <v>0.1</v>
-      </c>
-      <c r="AI11">
-        <v>1</v>
-      </c>
-      <c r="AJ11">
-        <v>0</v>
-      </c>
-      <c r="AK11">
-        <v>1</v>
-      </c>
-      <c r="AL11">
-        <v>0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
       <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
@@ -5923,7 +5414,7 @@
         <v>69</v>
       </c>
       <c r="F2">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G2">
         <v>0.9</v>
@@ -5967,16 +5458,16 @@
         <v>69</v>
       </c>
       <c r="F3">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G3">
         <v>0.9</v>
       </c>
       <c r="H3">
-        <v>1.0197000000000001</v>
+        <v>1.0197</v>
       </c>
       <c r="I3">
-        <v>-2.7981118567973098E-2</v>
+        <v>-0.0279811185679731</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -6011,16 +5502,16 @@
         <v>69</v>
       </c>
       <c r="F4">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G4">
         <v>0.9</v>
       </c>
       <c r="H4">
-        <v>1.0004200000000001</v>
+        <v>1.00042</v>
       </c>
       <c r="I4">
-        <v>-6.0096922133920698E-2</v>
+        <v>-0.0600969221339207</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -6055,16 +5546,16 @@
         <v>69</v>
       </c>
       <c r="F5">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G5">
         <v>0.9</v>
       </c>
       <c r="H5">
-        <v>0.99858000000000002</v>
+        <v>0.99858</v>
       </c>
       <c r="I5">
-        <v>-7.47210359363812E-2</v>
+        <v>-0.0747210359363812</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -6099,16 +5590,16 @@
         <v>69</v>
       </c>
       <c r="F6">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G6">
         <v>0.9</v>
       </c>
       <c r="H6">
-        <v>1.0044299999999999</v>
+        <v>1.00443</v>
       </c>
       <c r="I6">
-        <v>-6.4315382935990997E-2</v>
+        <v>-0.064315382935991</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -6143,16 +5634,16 @@
         <v>138</v>
       </c>
       <c r="F7">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G7">
         <v>0.9</v>
       </c>
       <c r="H7">
-        <v>0.99870999999999999</v>
+        <v>0.99871</v>
       </c>
       <c r="I7">
-        <v>-0.10999763077769099</v>
+        <v>-0.109997630777691</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -6187,7 +5678,7 @@
         <v>138</v>
       </c>
       <c r="F8">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G8">
         <v>0.9</v>
@@ -6196,7 +5687,7 @@
         <v>1.00682</v>
       </c>
       <c r="I8">
-        <v>-8.4285440237310202E-2</v>
+        <v>-0.0842854402373102</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -6231,7 +5722,7 @@
         <v>69</v>
       </c>
       <c r="F9">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G9">
         <v>0.9</v>
@@ -6240,7 +5731,7 @@
         <v>1.01895</v>
       </c>
       <c r="I9">
-        <v>-2.4338616419060901E-2</v>
+        <v>-0.0243386164190609</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -6275,7 +5766,7 @@
         <v>138</v>
       </c>
       <c r="F10">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G10">
         <v>0.9</v>
@@ -6284,7 +5775,7 @@
         <v>1.00193</v>
       </c>
       <c r="I10">
-        <v>-0.12750153784594201</v>
+        <v>-0.127501537845942</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -6319,7 +5810,7 @@
         <v>138</v>
       </c>
       <c r="F11">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G11">
         <v>0.9</v>
@@ -6328,7 +5819,7 @@
         <v>0.99351</v>
       </c>
       <c r="I11">
-        <v>-0.13020156219877699</v>
+        <v>-0.130201562198777</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -6363,13 +5854,13 @@
         <v>138</v>
       </c>
       <c r="F12">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G12">
         <v>0.9</v>
       </c>
       <c r="H12">
-        <v>0.99245000000000005</v>
+        <v>0.99245</v>
       </c>
       <c r="I12">
         <v>-0.122947973827489</v>
@@ -6407,13 +5898,13 @@
         <v>138</v>
       </c>
       <c r="F13">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G13">
         <v>0.9</v>
       </c>
       <c r="H13">
-        <v>0.98638999999999999</v>
+        <v>0.98639</v>
       </c>
       <c r="I13">
         <v>-0.128934453161829</v>
@@ -6451,16 +5942,16 @@
         <v>138</v>
       </c>
       <c r="F14">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G14">
         <v>0.9</v>
       </c>
       <c r="H14">
-        <v>0.98402999999999996</v>
+        <v>0.98403</v>
       </c>
       <c r="I14">
-        <v>-0.13378646848237299</v>
+        <v>-0.133786468482373</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -6495,13 +5986,13 @@
         <v>138</v>
       </c>
       <c r="F15">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G15">
         <v>0.9</v>
       </c>
       <c r="H15">
-        <v>0.99063000000000001</v>
+        <v>0.99063</v>
       </c>
       <c r="I15">
         <v>-0.16691630834373</v>
@@ -6524,19 +6015,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
@@ -6663,7 +6157,7 @@
         <v>69</v>
       </c>
       <c r="G4">
-        <v>0.47799999999999998</v>
+        <v>0.478</v>
       </c>
       <c r="H4">
         <v>0.1</v>
@@ -6698,10 +6192,10 @@
         <v>69</v>
       </c>
       <c r="G5">
-        <v>7.5999999999999998E-2</v>
+        <v>0.076</v>
       </c>
       <c r="H5">
-        <v>1.6E-2</v>
+        <v>0.016</v>
       </c>
       <c r="I5">
         <v>1.2</v>
@@ -6736,7 +6230,7 @@
         <v>0.15</v>
       </c>
       <c r="H6">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="I6">
         <v>1.2</v>
@@ -6768,10 +6262,10 @@
         <v>138</v>
       </c>
       <c r="G7">
-        <v>0.29499999999999998</v>
+        <v>0.295</v>
       </c>
       <c r="H7">
-        <v>0.16600000000000001</v>
+        <v>0.166</v>
       </c>
       <c r="I7">
         <v>1.2</v>
@@ -6806,7 +6300,7 @@
         <v>0.09</v>
       </c>
       <c r="H8">
-        <v>5.8000000000000003E-2</v>
+        <v>0.058</v>
       </c>
       <c r="I8">
         <v>1.2</v>
@@ -6838,10 +6332,10 @@
         <v>138</v>
       </c>
       <c r="G9">
-        <v>3.5000000000000003E-2</v>
+        <v>0.035</v>
       </c>
       <c r="H9">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="I9">
         <v>1.2</v>
@@ -6873,10 +6367,10 @@
         <v>138</v>
       </c>
       <c r="G10">
-        <v>6.0999999999999999E-2</v>
+        <v>0.061</v>
       </c>
       <c r="H10">
-        <v>1.6E-2</v>
+        <v>0.016</v>
       </c>
       <c r="I10">
         <v>1.2</v>
@@ -6908,10 +6402,10 @@
         <v>138</v>
       </c>
       <c r="G11">
-        <v>0.13500000000000001</v>
+        <v>0.135</v>
       </c>
       <c r="H11">
-        <v>5.8000000000000003E-2</v>
+        <v>0.058</v>
       </c>
       <c r="I11">
         <v>1.2</v>
@@ -6946,7 +6440,7 @@
         <v>0.2</v>
       </c>
       <c r="H12">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="I12">
         <v>1.2</v>
@@ -6960,19 +6454,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5"/>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
@@ -7315,19 +6812,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
@@ -7414,10 +6914,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0.81442000000000003</v>
+        <v>0.81442</v>
       </c>
       <c r="J2">
-        <v>1.9619999999999999E-2</v>
+        <v>0.01962</v>
       </c>
       <c r="K2">
         <v>2</v>
@@ -7452,19 +6952,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
@@ -7564,19 +7067,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
@@ -7652,7 +7158,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:21">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -7684,13 +7190,13 @@
         <v>69</v>
       </c>
       <c r="K2">
-        <v>1.9380000000000001E-2</v>
+        <v>0.01938</v>
       </c>
       <c r="L2">
-        <v>5.917E-2</v>
+        <v>0.05917</v>
       </c>
       <c r="M2">
-        <v>5.28E-2</v>
+        <v>0.0528</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -7717,7 +7223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:21">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -7749,13 +7255,13 @@
         <v>69</v>
       </c>
       <c r="K3">
-        <v>5.4030000000000002E-2</v>
+        <v>0.05403</v>
       </c>
       <c r="L3">
-        <v>0.22303999999999999</v>
+        <v>0.22304</v>
       </c>
       <c r="M3">
-        <v>4.9200000000000001E-2</v>
+        <v>0.0492</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -7782,7 +7288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:21">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -7814,13 +7320,13 @@
         <v>69</v>
       </c>
       <c r="K4">
-        <v>4.6989999999999997E-2</v>
+        <v>0.04699</v>
       </c>
       <c r="L4">
-        <v>0.19797000000000001</v>
+        <v>0.19797</v>
       </c>
       <c r="M4">
-        <v>4.3799999999999999E-2</v>
+        <v>0.0438</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -7847,7 +7353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:21">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -7879,13 +7385,13 @@
         <v>69</v>
       </c>
       <c r="K5">
-        <v>5.8110000000000002E-2</v>
+        <v>0.05811</v>
       </c>
       <c r="L5">
         <v>0.17632</v>
       </c>
       <c r="M5">
-        <v>3.4000000000000002E-2</v>
+        <v>0.034</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -7912,7 +7418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:21">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -7944,13 +7450,13 @@
         <v>69</v>
       </c>
       <c r="K6">
-        <v>5.6950000000000001E-2</v>
+        <v>0.05695</v>
       </c>
       <c r="L6">
-        <v>0.17388000000000001</v>
+        <v>0.17388</v>
       </c>
       <c r="M6">
-        <v>3.4599999999999999E-2</v>
+        <v>0.0346</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -7977,7 +7483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:21">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -8009,13 +7515,13 @@
         <v>69</v>
       </c>
       <c r="K7">
-        <v>6.701E-2</v>
+        <v>0.06701</v>
       </c>
       <c r="L7">
-        <v>0.17102999999999999</v>
+        <v>0.17103</v>
       </c>
       <c r="M7">
-        <v>1.2800000000000001E-2</v>
+        <v>0.0128</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -8042,7 +7548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:21">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -8074,10 +7580,10 @@
         <v>69</v>
       </c>
       <c r="K8">
-        <v>1.3350000000000001E-2</v>
+        <v>0.01335</v>
       </c>
       <c r="L8">
-        <v>4.2110000000000002E-2</v>
+        <v>0.04211</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -8107,7 +7613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:21">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -8139,10 +7645,10 @@
         <v>138</v>
       </c>
       <c r="K9">
-        <v>9.4979999999999995E-2</v>
+        <v>0.09498</v>
       </c>
       <c r="L9">
-        <v>0.19889999999999999</v>
+        <v>0.1989</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -8172,7 +7678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:21">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -8204,10 +7710,10 @@
         <v>138</v>
       </c>
       <c r="K10">
-        <v>0.12291000000000001</v>
+        <v>0.12291</v>
       </c>
       <c r="L10">
-        <v>0.25580999999999998</v>
+        <v>0.25581</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -8237,7 +7743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:21">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -8269,7 +7775,7 @@
         <v>138</v>
       </c>
       <c r="K11">
-        <v>6.615E-2</v>
+        <v>0.06615</v>
       </c>
       <c r="L11">
         <v>0.13027</v>
@@ -8302,7 +7808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:21">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -8367,7 +7873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:21">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -8399,10 +7905,10 @@
         <v>138</v>
       </c>
       <c r="K13">
-        <v>3.1809999999999998E-2</v>
+        <v>0.03181</v>
       </c>
       <c r="L13">
-        <v>8.4500000000000006E-2</v>
+        <v>0.0845</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -8432,7 +7938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:21">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -8467,7 +7973,7 @@
         <v>0.12711</v>
       </c>
       <c r="L14">
-        <v>0.27038000000000001</v>
+        <v>0.27038</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -8497,7 +8003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:21">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -8529,10 +8035,10 @@
         <v>138</v>
       </c>
       <c r="K15">
-        <v>8.2049999999999998E-2</v>
+        <v>0.08205</v>
       </c>
       <c r="L15">
-        <v>0.19206999999999999</v>
+        <v>0.19207</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -8562,7 +8068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:21">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -8594,7 +8100,7 @@
         <v>138</v>
       </c>
       <c r="K16">
-        <v>0.22092000000000001</v>
+        <v>0.22092</v>
       </c>
       <c r="L16">
         <v>0.19988</v>
@@ -8751,7 +8257,7 @@
         <v>1</v>
       </c>
       <c r="T18">
-        <v>0.99677000000000004</v>
+        <v>0.99677</v>
       </c>
       <c r="U18">
         <v>0</v>
@@ -8792,7 +8298,7 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>0.55618000000000001</v>
+        <v>0.55618</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -8816,7 +8322,7 @@
         <v>1</v>
       </c>
       <c r="T19">
-        <v>0.99677000000000004</v>
+        <v>0.99677</v>
       </c>
       <c r="U19">
         <v>0</v>
@@ -8857,7 +8363,7 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>0.25202000000000002</v>
+        <v>0.25202</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -8881,7 +8387,7 @@
         <v>1</v>
       </c>
       <c r="T20">
-        <v>0.99677000000000004</v>
+        <v>0.99677</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -8946,7 +8452,7 @@
         <v>1</v>
       </c>
       <c r="T21">
-        <v>0.99677000000000004</v>
+        <v>0.99677</v>
       </c>
       <c r="U21">
         <v>0</v>
@@ -8954,19 +8460,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -9012,5 +8521,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>